<commit_message>
Updated project management stuff and worked on turn test
</commit_message>
<xml_diff>
--- a/team_folder/newFolder/Project Management/Logging/Meeting Report.xlsx
+++ b/team_folder/newFolder/Project Management/Logging/Meeting Report.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>Cost</t>
   </si>
@@ -126,14 +126,33 @@
   </si>
   <si>
     <t xml:space="preserve">Reviewed what was completed, what the next tasks needed. Demo'd changes </t>
+  </si>
+  <si>
+    <t>Pre PDR Costs</t>
+  </si>
+  <si>
+    <t>Post PDR Costs</t>
+  </si>
+  <si>
+    <t>Pre PDR Hours</t>
+  </si>
+  <si>
+    <t>Post PDR Hours</t>
+  </si>
+  <si>
+    <t>Total Hours</t>
+  </si>
+  <si>
+    <t>Total Costs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -427,7 +446,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
@@ -493,6 +512,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="2" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency 2" xfId="3"/>
@@ -822,8 +843,9 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:AMK26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AL15" sqref="AL15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -837,18 +859,18 @@
     <col min="12" max="12" width="9.33203125" style="2" customWidth="1"/>
     <col min="13" max="14" width="8.6640625" style="2" customWidth="1"/>
     <col min="15" max="15" width="15" style="2" customWidth="1"/>
-    <col min="16" max="16" width="10.44140625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="8.88671875" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="21" width="10.44140625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="10.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="16" max="21" width="11.109375" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="11.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="19.6640625" style="2" customWidth="1"/>
-    <col min="24" max="29" width="8.6640625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="8.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="31" max="1025" width="8.6640625" style="2" customWidth="1"/>
+    <col min="24" max="29" width="8.6640625" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="31" width="8.6640625" style="2" customWidth="1"/>
+    <col min="32" max="32" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="1025" width="8.6640625" style="2" customWidth="1"/>
     <col min="1026" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="38"/>
       <c r="B1" s="37" t="s">
         <v>23</v>
@@ -870,7 +892,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>20</v>
       </c>
@@ -940,8 +962,26 @@
       <c r="AC2" s="22" t="s">
         <v>18</v>
       </c>
+      <c r="AG2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH2" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="27" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="26">
         <v>43132</v>
       </c>
@@ -1021,8 +1061,35 @@
         <f t="shared" ref="AC3:AC24" si="5">IF(I3=1,$C3,0)</f>
         <v>0.5</v>
       </c>
+      <c r="AF3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG3" s="39">
+        <f>SUM(P3:P14)</f>
+        <v>1075</v>
+      </c>
+      <c r="AH3" s="39">
+        <f t="shared" ref="AH3:AL3" si="6">SUM(Q3:Q14)</f>
+        <v>900</v>
+      </c>
+      <c r="AI3" s="39">
+        <f t="shared" si="6"/>
+        <v>1175</v>
+      </c>
+      <c r="AJ3" s="39">
+        <f t="shared" si="6"/>
+        <v>1175</v>
+      </c>
+      <c r="AK3" s="39">
+        <f t="shared" si="6"/>
+        <v>1175</v>
+      </c>
+      <c r="AL3" s="39">
+        <f t="shared" si="6"/>
+        <v>1175</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>43137</v>
       </c>
@@ -1049,36 +1116,36 @@
         <v>1</v>
       </c>
       <c r="J4" s="15">
-        <f t="shared" ref="J4:J24" si="6">SUM(D4:I4)*100*C4</f>
+        <f t="shared" ref="J4:J24" si="7">SUM(D4:I4)*100*C4</f>
         <v>300</v>
       </c>
       <c r="P4" s="9">
-        <f t="shared" ref="P4:P24" si="7">IF(D4=1,100*$C4,0)</f>
+        <f t="shared" ref="P4:P24" si="8">IF(D4=1,100*$C4,0)</f>
         <v>50</v>
       </c>
       <c r="Q4" s="9">
-        <f t="shared" ref="Q4:Q24" si="8">IF(E4=1,100*$C4,0)</f>
+        <f t="shared" ref="Q4:Q24" si="9">IF(E4=1,100*$C4,0)</f>
         <v>50</v>
       </c>
       <c r="R4" s="9">
-        <f t="shared" ref="R4:R24" si="9">IF(F4=1,100*$C4,0)</f>
+        <f t="shared" ref="R4:R24" si="10">IF(F4=1,100*$C4,0)</f>
         <v>50</v>
       </c>
       <c r="S4" s="9">
-        <f t="shared" ref="S4:S24" si="10">IF(G4=1,100*$C4,0)</f>
+        <f t="shared" ref="S4:S24" si="11">IF(G4=1,100*$C4,0)</f>
         <v>50</v>
       </c>
       <c r="T4" s="9">
-        <f t="shared" ref="T4:T24" si="11">IF(H4=1,100*$C4,0)</f>
+        <f t="shared" ref="T4:T24" si="12">IF(H4=1,100*$C4,0)</f>
         <v>50</v>
       </c>
       <c r="U4" s="9">
-        <f t="shared" ref="U4:U24" si="12">IF(I4=1,100*$C4,0)</f>
+        <f t="shared" ref="U4:U24" si="13">IF(I4=1,100*$C4,0)</f>
         <v>50</v>
       </c>
       <c r="V4" s="9"/>
       <c r="X4" s="2">
-        <f t="shared" ref="X4:X24" si="13">IF(D4=1,$C4,0)</f>
+        <f t="shared" ref="X4:X24" si="14">IF(D4=1,$C4,0)</f>
         <v>0.5</v>
       </c>
       <c r="Y4" s="2">
@@ -1101,8 +1168,35 @@
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
+      <c r="AF4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG4" s="40">
+        <f>P25-AG3</f>
+        <v>225</v>
+      </c>
+      <c r="AH4" s="40">
+        <f t="shared" ref="AH4:AL4" si="15">Q25-AH3</f>
+        <v>225</v>
+      </c>
+      <c r="AI4" s="40">
+        <f t="shared" si="15"/>
+        <v>225</v>
+      </c>
+      <c r="AJ4" s="40">
+        <f t="shared" si="15"/>
+        <v>225</v>
+      </c>
+      <c r="AK4" s="40">
+        <f t="shared" si="15"/>
+        <v>225</v>
+      </c>
+      <c r="AL4" s="40">
+        <f t="shared" si="15"/>
+        <v>225</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>43139</v>
       </c>
@@ -1129,36 +1223,36 @@
         <v>1</v>
       </c>
       <c r="J5" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>300</v>
       </c>
       <c r="P5" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="Q5" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="R5" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>50</v>
       </c>
       <c r="S5" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>50</v>
       </c>
       <c r="T5" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="U5" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="V5" s="9"/>
       <c r="X5" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="Y5" s="2">
@@ -1182,7 +1276,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>43144</v>
       </c>
@@ -1207,36 +1301,36 @@
         <v>1</v>
       </c>
       <c r="J6" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>375</v>
       </c>
       <c r="P6" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>75</v>
       </c>
       <c r="Q6" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R6" s="9">
-        <f t="shared" si="9"/>
-        <v>75</v>
-      </c>
-      <c r="S6" s="9">
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="T6" s="9">
+      <c r="S6" s="9">
         <f t="shared" si="11"/>
         <v>75</v>
       </c>
-      <c r="U6" s="9">
+      <c r="T6" s="9">
         <f t="shared" si="12"/>
         <v>75</v>
       </c>
+      <c r="U6" s="9">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
       <c r="V6" s="9"/>
       <c r="X6" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
       <c r="Y6" s="2">
@@ -1259,8 +1353,35 @@
         <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
+      <c r="AF6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG6" s="2">
+        <f>SUM(X3:X14)</f>
+        <v>10.75</v>
+      </c>
+      <c r="AH6" s="2">
+        <f t="shared" ref="AH6:AL6" si="16">SUM(Y3:Y14)</f>
+        <v>9</v>
+      </c>
+      <c r="AI6" s="2">
+        <f t="shared" si="16"/>
+        <v>11.75</v>
+      </c>
+      <c r="AJ6" s="2">
+        <f t="shared" si="16"/>
+        <v>11.75</v>
+      </c>
+      <c r="AK6" s="2">
+        <f t="shared" si="16"/>
+        <v>11.75</v>
+      </c>
+      <c r="AL6" s="2">
+        <f t="shared" si="16"/>
+        <v>11.75</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>43151</v>
       </c>
@@ -1289,36 +1410,36 @@
         <v>1</v>
       </c>
       <c r="J7" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>600</v>
       </c>
       <c r="P7" s="9">
-        <f t="shared" si="7"/>
-        <v>100</v>
-      </c>
-      <c r="Q7" s="9">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="R7" s="9">
+      <c r="Q7" s="9">
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="S7" s="9">
+      <c r="R7" s="9">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="T7" s="9">
+      <c r="S7" s="9">
         <f t="shared" si="11"/>
         <v>100</v>
       </c>
-      <c r="U7" s="9">
+      <c r="T7" s="9">
         <f t="shared" si="12"/>
         <v>100</v>
       </c>
+      <c r="U7" s="9">
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
       <c r="V7" s="9"/>
       <c r="X7" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="Y7" s="2">
@@ -1341,8 +1462,35 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
+      <c r="AF7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG7" s="2">
+        <f>X25-AG6</f>
+        <v>2.25</v>
+      </c>
+      <c r="AH7" s="2">
+        <f t="shared" ref="AH7:AL7" si="17">Y25-AH6</f>
+        <v>2.25</v>
+      </c>
+      <c r="AI7" s="2">
+        <f t="shared" si="17"/>
+        <v>2.25</v>
+      </c>
+      <c r="AJ7" s="2">
+        <f t="shared" si="17"/>
+        <v>2.25</v>
+      </c>
+      <c r="AK7" s="2">
+        <f t="shared" si="17"/>
+        <v>2.25</v>
+      </c>
+      <c r="AL7" s="2">
+        <f t="shared" si="17"/>
+        <v>2.25</v>
+      </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>43153</v>
       </c>
@@ -1369,36 +1517,36 @@
         <v>1</v>
       </c>
       <c r="J8" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>500</v>
       </c>
       <c r="P8" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q8" s="9">
-        <f t="shared" si="8"/>
-        <v>100</v>
-      </c>
-      <c r="R8" s="9">
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="S8" s="9">
+      <c r="R8" s="9">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="T8" s="9">
+      <c r="S8" s="9">
         <f t="shared" si="11"/>
         <v>100</v>
       </c>
-      <c r="U8" s="9">
+      <c r="T8" s="9">
         <f t="shared" si="12"/>
         <v>100</v>
       </c>
+      <c r="U8" s="9">
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
       <c r="V8" s="9"/>
       <c r="X8" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y8" s="2">
@@ -1422,7 +1570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>43158</v>
       </c>
@@ -1451,36 +1599,36 @@
         <v>1</v>
       </c>
       <c r="J9" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>900</v>
       </c>
       <c r="P9" s="9">
-        <f t="shared" si="7"/>
-        <v>150</v>
-      </c>
-      <c r="Q9" s="9">
         <f t="shared" si="8"/>
         <v>150</v>
       </c>
-      <c r="R9" s="9">
+      <c r="Q9" s="9">
         <f t="shared" si="9"/>
         <v>150</v>
       </c>
-      <c r="S9" s="9">
+      <c r="R9" s="9">
         <f t="shared" si="10"/>
         <v>150</v>
       </c>
-      <c r="T9" s="9">
+      <c r="S9" s="9">
         <f t="shared" si="11"/>
         <v>150</v>
       </c>
-      <c r="U9" s="9">
+      <c r="T9" s="9">
         <f t="shared" si="12"/>
         <v>150</v>
       </c>
+      <c r="U9" s="9">
+        <f t="shared" si="13"/>
+        <v>150</v>
+      </c>
       <c r="V9" s="9"/>
       <c r="X9" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.5</v>
       </c>
       <c r="Y9" s="2">
@@ -1503,8 +1651,35 @@
         <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
+      <c r="AF9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG9" s="39">
+        <f>SUM(AG3,AG4)</f>
+        <v>1300</v>
+      </c>
+      <c r="AH9" s="39">
+        <f t="shared" ref="AH9:AL9" si="18">SUM(AH3,AH4)</f>
+        <v>1125</v>
+      </c>
+      <c r="AI9" s="39">
+        <f t="shared" si="18"/>
+        <v>1400</v>
+      </c>
+      <c r="AJ9" s="39">
+        <f t="shared" si="18"/>
+        <v>1400</v>
+      </c>
+      <c r="AK9" s="39">
+        <f t="shared" si="18"/>
+        <v>1400</v>
+      </c>
+      <c r="AL9" s="39">
+        <f t="shared" si="18"/>
+        <v>1400</v>
+      </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>43160</v>
       </c>
@@ -1533,36 +1708,36 @@
         <v>1</v>
       </c>
       <c r="J10" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1200</v>
       </c>
       <c r="P10" s="9">
-        <f t="shared" si="7"/>
-        <v>200</v>
-      </c>
-      <c r="Q10" s="9">
         <f t="shared" si="8"/>
         <v>200</v>
       </c>
-      <c r="R10" s="9">
+      <c r="Q10" s="9">
         <f t="shared" si="9"/>
         <v>200</v>
       </c>
-      <c r="S10" s="9">
+      <c r="R10" s="9">
         <f t="shared" si="10"/>
         <v>200</v>
       </c>
-      <c r="T10" s="9">
+      <c r="S10" s="9">
         <f t="shared" si="11"/>
         <v>200</v>
       </c>
-      <c r="U10" s="9">
+      <c r="T10" s="9">
         <f t="shared" si="12"/>
         <v>200</v>
       </c>
+      <c r="U10" s="9">
+        <f t="shared" si="13"/>
+        <v>200</v>
+      </c>
       <c r="V10" s="9"/>
       <c r="X10" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="Y10" s="2">
@@ -1585,8 +1760,35 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
+      <c r="AF10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG10" s="2">
+        <f>SUM(AG6+AG7)</f>
+        <v>13</v>
+      </c>
+      <c r="AH10" s="2">
+        <f t="shared" ref="AH10:AL10" si="19">SUM(AH6+AH7)</f>
+        <v>11.25</v>
+      </c>
+      <c r="AI10" s="2">
+        <f t="shared" si="19"/>
+        <v>14</v>
+      </c>
+      <c r="AJ10" s="2">
+        <f t="shared" si="19"/>
+        <v>14</v>
+      </c>
+      <c r="AK10" s="2">
+        <f t="shared" si="19"/>
+        <v>14</v>
+      </c>
+      <c r="AL10" s="2">
+        <f t="shared" si="19"/>
+        <v>14</v>
+      </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>43164</v>
       </c>
@@ -1615,36 +1817,36 @@
         <v>1</v>
       </c>
       <c r="J11" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>300</v>
       </c>
       <c r="P11" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="Q11" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="R11" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>50</v>
       </c>
       <c r="S11" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>50</v>
       </c>
       <c r="T11" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="U11" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="V11" s="9"/>
       <c r="X11" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="Y11" s="2">
@@ -1668,7 +1870,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>43165</v>
       </c>
@@ -1697,36 +1899,36 @@
         <v>1</v>
       </c>
       <c r="J12" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>600</v>
       </c>
       <c r="P12" s="9">
-        <f t="shared" si="7"/>
-        <v>100</v>
-      </c>
-      <c r="Q12" s="9">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="R12" s="9">
+      <c r="Q12" s="9">
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="S12" s="9">
+      <c r="R12" s="9">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="T12" s="9">
+      <c r="S12" s="9">
         <f t="shared" si="11"/>
         <v>100</v>
       </c>
-      <c r="U12" s="9">
+      <c r="T12" s="9">
         <f t="shared" si="12"/>
         <v>100</v>
       </c>
+      <c r="U12" s="9">
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
       <c r="V12" s="9"/>
       <c r="X12" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="Y12" s="2">
@@ -1750,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>43167</v>
       </c>
@@ -1779,36 +1981,36 @@
         <v>1</v>
       </c>
       <c r="J13" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>300</v>
       </c>
       <c r="P13" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="Q13" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="R13" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>50</v>
       </c>
       <c r="S13" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>50</v>
       </c>
       <c r="T13" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="U13" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="V13" s="9"/>
       <c r="X13" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="Y13" s="2">
@@ -1832,7 +2034,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>43179</v>
       </c>
@@ -1859,36 +2061,36 @@
         <v>1</v>
       </c>
       <c r="J14" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1000</v>
       </c>
       <c r="P14" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>200</v>
       </c>
       <c r="Q14" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R14" s="9">
-        <f t="shared" si="9"/>
-        <v>200</v>
-      </c>
-      <c r="S14" s="9">
         <f t="shared" si="10"/>
         <v>200</v>
       </c>
-      <c r="T14" s="9">
+      <c r="S14" s="9">
         <f t="shared" si="11"/>
         <v>200</v>
       </c>
-      <c r="U14" s="9">
+      <c r="T14" s="9">
         <f t="shared" si="12"/>
         <v>200</v>
       </c>
+      <c r="U14" s="9">
+        <f t="shared" si="13"/>
+        <v>200</v>
+      </c>
       <c r="V14" s="9"/>
       <c r="X14" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="Y14" s="2">
@@ -1912,7 +2114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>43186</v>
       </c>
@@ -1941,36 +2143,36 @@
         <v>1</v>
       </c>
       <c r="J15" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>300</v>
       </c>
       <c r="P15" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="Q15" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="R15" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>50</v>
       </c>
       <c r="S15" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>50</v>
       </c>
       <c r="T15" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="U15" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="V15" s="9"/>
       <c r="X15" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="Y15" s="2">
@@ -1994,7 +2196,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" ht="27" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>43195</v>
       </c>
@@ -2023,36 +2225,36 @@
         <v>1</v>
       </c>
       <c r="J16" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>600</v>
       </c>
       <c r="P16" s="9">
-        <f t="shared" si="7"/>
-        <v>100</v>
-      </c>
-      <c r="Q16" s="9">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="R16" s="9">
+      <c r="Q16" s="9">
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="S16" s="9">
+      <c r="R16" s="9">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="T16" s="9">
+      <c r="S16" s="9">
         <f t="shared" si="11"/>
         <v>100</v>
       </c>
-      <c r="U16" s="9">
+      <c r="T16" s="9">
         <f t="shared" si="12"/>
         <v>100</v>
       </c>
+      <c r="U16" s="9">
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
       <c r="V16" s="9"/>
       <c r="X16" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="Y16" s="2">
@@ -2105,36 +2307,36 @@
         <v>1</v>
       </c>
       <c r="J17" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>450</v>
       </c>
       <c r="P17" s="9">
-        <f t="shared" si="7"/>
-        <v>75</v>
-      </c>
-      <c r="Q17" s="9">
         <f t="shared" si="8"/>
         <v>75</v>
       </c>
-      <c r="R17" s="9">
+      <c r="Q17" s="9">
         <f t="shared" si="9"/>
         <v>75</v>
       </c>
-      <c r="S17" s="9">
+      <c r="R17" s="9">
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="T17" s="9">
+      <c r="S17" s="9">
         <f t="shared" si="11"/>
         <v>75</v>
       </c>
-      <c r="U17" s="9">
+      <c r="T17" s="9">
         <f t="shared" si="12"/>
         <v>75</v>
       </c>
+      <c r="U17" s="9">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
       <c r="V17" s="9"/>
       <c r="X17" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
       <c r="Y17" s="2">
@@ -2169,36 +2371,36 @@
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
       <c r="J18" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P18" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q18" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R18" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S18" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T18" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U18" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="V18" s="9"/>
       <c r="X18" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y18" s="2">
@@ -2233,36 +2435,36 @@
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
       <c r="J19" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P19" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q19" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R19" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S19" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T19" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U19" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="V19" s="9"/>
       <c r="X19" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y19" s="2">
@@ -2297,36 +2499,36 @@
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
       <c r="J20" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P20" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q20" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R20" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S20" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T20" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U20" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="V20" s="9"/>
       <c r="X20" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y20" s="2">
@@ -2361,36 +2563,36 @@
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
       <c r="J21" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P21" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q21" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R21" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S21" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T21" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U21" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="V21" s="9"/>
       <c r="X21" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y21" s="2">
@@ -2425,36 +2627,36 @@
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
       <c r="J22" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P22" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q22" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R22" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S22" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T22" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U22" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="V22" s="9"/>
       <c r="X22" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y22" s="2">
@@ -2489,36 +2691,36 @@
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
       <c r="J23" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P23" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q23" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R23" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S23" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T23" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U23" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="V23" s="9"/>
       <c r="X23" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y23" s="2">
@@ -2553,36 +2755,36 @@
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
       <c r="J24" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P24" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q24" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R24" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S24" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T24" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U24" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="V24" s="9"/>
       <c r="X24" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y24" s="2">
@@ -2616,27 +2818,27 @@
         <v>14</v>
       </c>
       <c r="D25" s="11">
-        <f t="shared" ref="D25:I25" si="14">X$25</f>
+        <f t="shared" ref="D25:I25" si="20">X$25</f>
         <v>13</v>
       </c>
       <c r="E25" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>11.25</v>
       </c>
       <c r="F25" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14</v>
       </c>
       <c r="G25" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14</v>
       </c>
       <c r="H25" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14</v>
       </c>
       <c r="I25" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>14</v>
       </c>
       <c r="J25" s="10">
@@ -2647,27 +2849,27 @@
         <v>8</v>
       </c>
       <c r="P25" s="9">
-        <f t="shared" ref="P25:U25" si="15">SUM(P3:P24)</f>
+        <f t="shared" ref="P25:U25" si="21">SUM(P3:P24)</f>
         <v>1300</v>
       </c>
       <c r="Q25" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1125</v>
       </c>
       <c r="R25" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1400</v>
       </c>
       <c r="S25" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1400</v>
       </c>
       <c r="T25" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1400</v>
       </c>
       <c r="U25" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1400</v>
       </c>
       <c r="V25" s="9">
@@ -2675,27 +2877,27 @@
         <v>8025</v>
       </c>
       <c r="X25" s="2">
-        <f t="shared" ref="X25:AC25" si="16">SUM(X3:X24)</f>
+        <f t="shared" ref="X25:AC25" si="22">SUM(X3:X24)</f>
         <v>13</v>
       </c>
       <c r="Y25" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>11.25</v>
       </c>
       <c r="Z25" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>14</v>
       </c>
       <c r="AA25" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>14</v>
       </c>
       <c r="AB25" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>14</v>
       </c>
       <c r="AC25" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>14</v>
       </c>
       <c r="AD25" s="2">

</xml_diff>

<commit_message>
Refactor of IMU test and synced share
</commit_message>
<xml_diff>
--- a/team_folder/newFolder/Project Management/Logging/Meeting Report.xlsx
+++ b/team_folder/newFolder/Project Management/Logging/Meeting Report.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\groups\newFolder\Project Management\Logging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\soet-students\courses\CPET-563\groups\newFolder\Project Management\Logging\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Meeting Costs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <definedName name="TitleRegion..BO60">#REF!</definedName>
     <definedName name="Um">PeriodInPlan*(#REF!&gt;0)</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" calcMode="manual" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -149,10 +149,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -513,7 +513,7 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency 2" xfId="3"/>
@@ -844,33 +844,34 @@
   <dimension ref="A1:AMK26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL15" sqref="AL15"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="2" customWidth="1"/>
     <col min="4" max="9" width="9" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" style="2" customWidth="1"/>
-    <col min="13" max="14" width="8.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" style="2" customWidth="1"/>
+    <col min="13" max="14" width="8.7109375" style="2" customWidth="1"/>
     <col min="15" max="15" width="15" style="2" customWidth="1"/>
-    <col min="16" max="21" width="11.109375" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="11.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="19.6640625" style="2" customWidth="1"/>
-    <col min="24" max="29" width="8.6640625" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="31" width="8.6640625" style="2" customWidth="1"/>
-    <col min="32" max="32" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="1025" width="8.6640625" style="2" customWidth="1"/>
-    <col min="1026" max="16384" width="8.88671875" style="1"/>
+    <col min="16" max="21" width="11.140625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="11.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19.7109375" style="2" customWidth="1"/>
+    <col min="24" max="29" width="8.7109375" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="8.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="8.7109375" style="2" customWidth="1"/>
+    <col min="32" max="32" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="1025" width="8.7109375" style="2" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38"/>
       <c r="B1" s="37" t="s">
         <v>23</v>
@@ -892,7 +893,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>20</v>
       </c>
@@ -981,7 +982,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="26">
         <v>43132</v>
       </c>
@@ -1089,7 +1090,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>43137</v>
       </c>
@@ -1173,7 +1174,7 @@
       </c>
       <c r="AG4" s="40">
         <f>P25-AG3</f>
-        <v>225</v>
+        <v>275</v>
       </c>
       <c r="AH4" s="40">
         <f t="shared" ref="AH4:AL4" si="15">Q25-AH3</f>
@@ -1181,22 +1182,22 @@
       </c>
       <c r="AI4" s="40">
         <f t="shared" si="15"/>
-        <v>225</v>
+        <v>275</v>
       </c>
       <c r="AJ4" s="40">
         <f t="shared" si="15"/>
-        <v>225</v>
+        <v>275</v>
       </c>
       <c r="AK4" s="40">
         <f t="shared" si="15"/>
-        <v>225</v>
+        <v>275</v>
       </c>
       <c r="AL4" s="40">
         <f t="shared" si="15"/>
-        <v>225</v>
+        <v>275</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>43139</v>
       </c>
@@ -1276,7 +1277,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>43144</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>43151</v>
       </c>
@@ -1467,7 +1468,7 @@
       </c>
       <c r="AG7" s="2">
         <f>X25-AG6</f>
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="AH7" s="2">
         <f t="shared" ref="AH7:AL7" si="17">Y25-AH6</f>
@@ -1475,22 +1476,22 @@
       </c>
       <c r="AI7" s="2">
         <f t="shared" si="17"/>
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="AJ7" s="2">
         <f t="shared" si="17"/>
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="AK7" s="2">
         <f t="shared" si="17"/>
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="AL7" s="2">
         <f t="shared" si="17"/>
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>43153</v>
       </c>
@@ -1570,7 +1571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>43158</v>
       </c>
@@ -1656,7 +1657,7 @@
       </c>
       <c r="AG9" s="39">
         <f>SUM(AG3,AG4)</f>
-        <v>1300</v>
+        <v>1350</v>
       </c>
       <c r="AH9" s="39">
         <f t="shared" ref="AH9:AL9" si="18">SUM(AH3,AH4)</f>
@@ -1664,22 +1665,22 @@
       </c>
       <c r="AI9" s="39">
         <f t="shared" si="18"/>
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="AJ9" s="39">
         <f t="shared" si="18"/>
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="AK9" s="39">
         <f t="shared" si="18"/>
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="AL9" s="39">
         <f t="shared" si="18"/>
-        <v>1400</v>
+        <v>1450</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>43160</v>
       </c>
@@ -1765,7 +1766,7 @@
       </c>
       <c r="AG10" s="2">
         <f>SUM(AG6+AG7)</f>
-        <v>13</v>
+        <v>13.5</v>
       </c>
       <c r="AH10" s="2">
         <f t="shared" ref="AH10:AL10" si="19">SUM(AH6+AH7)</f>
@@ -1773,22 +1774,22 @@
       </c>
       <c r="AI10" s="2">
         <f t="shared" si="19"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="AJ10" s="2">
         <f t="shared" si="19"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="AK10" s="2">
         <f t="shared" si="19"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="AL10" s="2">
         <f t="shared" si="19"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>43164</v>
       </c>
@@ -1870,7 +1871,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>43165</v>
       </c>
@@ -1952,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>43167</v>
       </c>
@@ -2034,7 +2035,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>43179</v>
       </c>
@@ -2114,7 +2115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>43186</v>
       </c>
@@ -2196,7 +2197,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>43195</v>
       </c>
@@ -2278,7 +2279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>43200</v>
       </c>
@@ -2360,23 +2361,37 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="19">
+        <v>43202</v>
+      </c>
       <c r="B18" s="18"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="16"/>
+      <c r="C18" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
       <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
+      <c r="F18" s="16">
+        <v>1</v>
+      </c>
+      <c r="G18" s="16">
+        <v>1</v>
+      </c>
+      <c r="H18" s="16">
+        <v>1</v>
+      </c>
+      <c r="I18" s="16">
+        <v>1</v>
+      </c>
       <c r="J18" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>SUM(D18:I18)*100*C18</f>
+        <v>250</v>
       </c>
       <c r="P18" s="9">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Q18" s="9">
         <f t="shared" si="9"/>
@@ -2384,24 +2399,24 @@
       </c>
       <c r="R18" s="9">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="S18" s="9">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="T18" s="9">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="U18" s="9">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="V18" s="9"/>
       <c r="X18" s="2">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y18" s="2">
         <f t="shared" si="1"/>
@@ -2409,22 +2424,22 @@
       </c>
       <c r="Z18" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AA18" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AB18" s="2">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AC18" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="18"/>
       <c r="C19" s="20"/>
@@ -2488,7 +2503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="18"/>
       <c r="C20" s="20"/>
@@ -2552,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="18"/>
       <c r="C21" s="20"/>
@@ -2616,7 +2631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="18"/>
       <c r="C22" s="20"/>
@@ -2680,7 +2695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="18"/>
       <c r="C23" s="20"/>
@@ -2744,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="18"/>
       <c r="C24" s="17"/>
@@ -2808,18 +2823,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="12">
         <f>SUM(C3:C24)</f>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="D25" s="11">
         <f t="shared" ref="D25:I25" si="20">X$25</f>
-        <v>13</v>
+        <v>13.5</v>
       </c>
       <c r="E25" s="11">
         <f t="shared" si="20"/>
@@ -2827,30 +2842,30 @@
       </c>
       <c r="F25" s="11">
         <f t="shared" si="20"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="G25" s="11">
         <f t="shared" si="20"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="H25" s="11">
         <f t="shared" si="20"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="I25" s="11">
         <f t="shared" si="20"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="J25" s="10">
         <f>SUM(J3:J24)</f>
-        <v>8025</v>
+        <v>8275</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="P25" s="9">
         <f t="shared" ref="P25:U25" si="21">SUM(P3:P24)</f>
-        <v>1300</v>
+        <v>1350</v>
       </c>
       <c r="Q25" s="9">
         <f t="shared" si="21"/>
@@ -2858,27 +2873,27 @@
       </c>
       <c r="R25" s="9">
         <f t="shared" si="21"/>
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="S25" s="9">
         <f t="shared" si="21"/>
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="T25" s="9">
         <f t="shared" si="21"/>
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="U25" s="9">
         <f t="shared" si="21"/>
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="V25" s="9">
         <f>SUM(P25:U25)</f>
-        <v>8025</v>
+        <v>8275</v>
       </c>
       <c r="X25" s="2">
         <f t="shared" ref="X25:AC25" si="22">SUM(X3:X24)</f>
-        <v>13</v>
+        <v>13.5</v>
       </c>
       <c r="Y25" s="2">
         <f t="shared" si="22"/>
@@ -2886,26 +2901,26 @@
       </c>
       <c r="Z25" s="2">
         <f t="shared" si="22"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="AA25" s="2">
         <f t="shared" si="22"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="AB25" s="2">
         <f t="shared" si="22"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="AC25" s="2">
         <f t="shared" si="22"/>
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="AD25" s="2">
         <f>SUM(X25:AC25)</f>
-        <v>80.25</v>
+        <v>82.75</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="7" t="s">
         <v>7</v>

</xml_diff>